<commit_message>
modified based on Pavans File
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1466EE7-44B5-40C8-80A7-A8EA2A3418D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966F2A21-D4E5-48B9-B56B-843354DF8F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -28,38 +28,32 @@
     <t>password</t>
   </si>
   <si>
+    <t xml:space="preserve">admin@yourstore.com </t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>adm</t>
+  </si>
+  <si>
+    <t>adm@yourstore.com</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>exp</t>
-  </si>
-  <si>
-    <t>admin@yourstore.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>admin1@yourstore.com</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin2@yourstore.com</t>
-  </si>
-  <si>
-    <t>newadmin</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +69,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,14 +115,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -161,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -194,9 +240,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -229,6 +292,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -384,77 +464,79 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6:U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C11386AC-9E47-4C5F-A26E-F51DB922BA84}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{062F86A7-70CC-42E5-9B14-275A4C76AE4F}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{028FB11A-AD22-4C7E-A4C1-6F4B68F0416A}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{BA081438-4862-4DBB-9854-71A5FB2BD3FB}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7ED63F57-644F-4E78-9587-08CB51DEF5FB}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{EB480860-584A-43F6-9478-DD4F2553FE6D}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{EB701B42-A320-4932-9568-F231C8F446AB}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{716734F3-6854-43CF-931C-C8D1149FAF15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>